<commit_message>
ready for exc 3
</commit_message>
<xml_diff>
--- a/_other/_8_drills-step analysis-01.xlsx
+++ b/_other/_8_drills-step analysis-01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19260" windowHeight="1320" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19260" windowHeight="1320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -13531,7 +13531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM262"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -26241,11 +26241,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL261"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -37453,7 +37453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>